<commit_message>
updated prisons template (#351)
</commit_message>
<xml_diff>
--- a/publisher/public/assets/PRISONS.xlsx
+++ b/publisher/public/assets/PRISONS.xlsx
@@ -11,8 +11,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="funding_by_type" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="expenses" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="expenses_by_type" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="total_staff" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="total_staff_by_type" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="staff" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="staff_by_type" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="readmissions" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="readmissions_by_type" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="admissions" sheetId="9" state="visible" r:id="rId9"/>
@@ -24,9 +24,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="releases" sheetId="15" state="visible" r:id="rId15"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="releases_by_type" sheetId="16" state="visible" r:id="rId16"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="use_of_force" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="use_of_force_by_type" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grievances_upheld" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grievances_upheld_by_type" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grievances_upheld" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="grievances_upheld_by_type" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18242,7 +18241,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -18260,7 +18259,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -18278,7 +18277,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -18296,7 +18295,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -18314,7 +18313,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -18332,7 +18331,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -18350,7 +18349,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -18368,7 +18367,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -18386,7 +18385,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -18404,7 +18403,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -18422,7 +18421,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -18440,7 +18439,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -18458,7 +18457,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -18476,7 +18475,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -18494,7 +18493,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -18512,7 +18511,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -18530,7 +18529,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -18548,7 +18547,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -18566,7 +18565,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -18584,7 +18583,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -18602,7 +18601,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -18620,7 +18619,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -18638,7 +18637,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -18656,7 +18655,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -18674,7 +18673,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -18692,7 +18691,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -18710,7 +18709,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -18728,7 +18727,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -18746,7 +18745,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -18764,7 +18763,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -18782,7 +18781,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -18800,7 +18799,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -18818,7 +18817,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -18836,7 +18835,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -18854,7 +18853,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -18872,7 +18871,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -18890,7 +18889,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -18908,7 +18907,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -18926,7 +18925,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -18944,7 +18943,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -18962,7 +18961,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -18980,7 +18979,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -18998,7 +18997,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -19016,7 +19015,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -19034,7 +19033,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -19052,7 +19051,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
@@ -19070,7 +19069,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
@@ -19088,7 +19087,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
@@ -19106,7 +19105,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
@@ -19124,7 +19123,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
@@ -19142,7 +19141,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
@@ -19160,7 +19159,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
@@ -19178,7 +19177,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
@@ -19196,7 +19195,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
@@ -19214,7 +19213,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
@@ -19232,7 +19231,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
@@ -19250,7 +19249,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
@@ -19268,7 +19267,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
@@ -19286,7 +19285,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
@@ -19304,7 +19303,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
@@ -19322,7 +19321,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
@@ -19340,7 +19339,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
@@ -19358,7 +19357,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
@@ -19376,7 +19375,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
@@ -19394,7 +19393,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
@@ -19412,7 +19411,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
@@ -19430,7 +19429,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
@@ -19448,7 +19447,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
@@ -19466,7 +19465,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
@@ -19484,7 +19483,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
@@ -19502,7 +19501,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
@@ -19520,7 +19519,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
@@ -19538,7 +19537,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
@@ -19556,7 +19555,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
@@ -19574,7 +19573,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
@@ -19592,7 +19591,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
@@ -19610,7 +19609,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
@@ -19628,7 +19627,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
@@ -19646,7 +19645,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
@@ -19664,7 +19663,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
@@ -19682,7 +19681,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
@@ -19700,7 +19699,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
@@ -19718,7 +19717,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
@@ -19736,7 +19735,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
@@ -19754,7 +19753,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D86" t="inlineStr"/>
@@ -19772,7 +19771,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
@@ -19790,7 +19789,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
@@ -19808,7 +19807,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D89" t="inlineStr"/>
@@ -19826,7 +19825,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D90" t="inlineStr"/>
@@ -19844,7 +19843,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D91" t="inlineStr"/>
@@ -19862,7 +19861,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D92" t="inlineStr"/>
@@ -19880,7 +19879,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D93" t="inlineStr"/>
@@ -19898,7 +19897,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D94" t="inlineStr"/>
@@ -19916,7 +19915,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D95" t="inlineStr"/>
@@ -19934,7 +19933,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
@@ -19952,7 +19951,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
@@ -19970,7 +19969,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D98" t="inlineStr"/>
@@ -19988,7 +19987,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D99" t="inlineStr"/>
@@ -20006,7 +20005,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
@@ -20024,7 +20023,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
@@ -20042,7 +20041,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D102" t="inlineStr"/>
@@ -20060,7 +20059,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D103" t="inlineStr"/>
@@ -20078,7 +20077,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D104" t="inlineStr"/>
@@ -20096,7 +20095,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D105" t="inlineStr"/>
@@ -20114,7 +20113,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
@@ -20132,7 +20131,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D107" t="inlineStr"/>
@@ -20150,7 +20149,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D108" t="inlineStr"/>
@@ -20168,7 +20167,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D109" t="inlineStr"/>
@@ -20186,7 +20185,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D110" t="inlineStr"/>
@@ -20204,7 +20203,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D111" t="inlineStr"/>
@@ -20222,7 +20221,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D112" t="inlineStr"/>
@@ -20240,7 +20239,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D113" t="inlineStr"/>
@@ -20258,7 +20257,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D114" t="inlineStr"/>
@@ -20276,7 +20275,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D115" t="inlineStr"/>
@@ -20294,7 +20293,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D116" t="inlineStr"/>
@@ -20312,7 +20311,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D117" t="inlineStr"/>
@@ -20330,7 +20329,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D118" t="inlineStr"/>
@@ -20348,7 +20347,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D119" t="inlineStr"/>
@@ -20366,7 +20365,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D120" t="inlineStr"/>
@@ -20384,7 +20383,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D121" t="inlineStr"/>
@@ -20402,7 +20401,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D122" t="inlineStr"/>
@@ -20420,7 +20419,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D123" t="inlineStr"/>
@@ -20438,7 +20437,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D124" t="inlineStr"/>
@@ -20456,7 +20455,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D125" t="inlineStr"/>
@@ -20474,7 +20473,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D126" t="inlineStr"/>
@@ -20492,7 +20491,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D127" t="inlineStr"/>
@@ -20510,7 +20509,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D128" t="inlineStr"/>
@@ -20528,7 +20527,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D129" t="inlineStr"/>
@@ -20546,7 +20545,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D130" t="inlineStr"/>
@@ -20564,7 +20563,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D131" t="inlineStr"/>
@@ -20582,7 +20581,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D132" t="inlineStr"/>
@@ -20600,7 +20599,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D133" t="inlineStr"/>
@@ -20618,7 +20617,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D134" t="inlineStr"/>
@@ -20636,7 +20635,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D135" t="inlineStr"/>
@@ -20654,7 +20653,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D136" t="inlineStr"/>
@@ -20672,7 +20671,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D137" t="inlineStr"/>
@@ -20690,7 +20689,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D138" t="inlineStr"/>
@@ -20708,7 +20707,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D139" t="inlineStr"/>
@@ -20726,7 +20725,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D140" t="inlineStr"/>
@@ -20744,7 +20743,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D141" t="inlineStr"/>
@@ -20762,7 +20761,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D142" t="inlineStr"/>
@@ -20780,7 +20779,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D143" t="inlineStr"/>
@@ -20798,7 +20797,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D144" t="inlineStr"/>
@@ -20816,7 +20815,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D145" t="inlineStr"/>
@@ -20834,7 +20833,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D146" t="inlineStr"/>
@@ -20852,7 +20851,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D147" t="inlineStr"/>
@@ -20870,7 +20869,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D148" t="inlineStr"/>
@@ -20888,7 +20887,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D149" t="inlineStr"/>
@@ -20906,7 +20905,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D150" t="inlineStr"/>
@@ -20924,7 +20923,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D151" t="inlineStr"/>
@@ -20942,7 +20941,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D152" t="inlineStr"/>
@@ -20960,7 +20959,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D153" t="inlineStr"/>
@@ -20978,7 +20977,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D154" t="inlineStr"/>
@@ -20996,7 +20995,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D155" t="inlineStr"/>
@@ -21014,7 +21013,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D156" t="inlineStr"/>
@@ -21032,7 +21031,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D157" t="inlineStr"/>
@@ -21050,7 +21049,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D158" t="inlineStr"/>
@@ -21068,7 +21067,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D159" t="inlineStr"/>
@@ -21086,7 +21085,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D160" t="inlineStr"/>
@@ -21104,7 +21103,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D161" t="inlineStr"/>
@@ -21122,7 +21121,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D162" t="inlineStr"/>
@@ -21140,7 +21139,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>To Parole Supervision</t>
+          <t>Releases from Prison to Probation Supervision</t>
         </is>
       </c>
       <c r="D163" t="inlineStr"/>
@@ -21158,7 +21157,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>To Probation Supervision</t>
+          <t>Releases from Prison to Parole Supervision</t>
         </is>
       </c>
       <c r="D164" t="inlineStr"/>
@@ -21176,7 +21175,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>To Other Community Supervision That Is Not Probation or Parole</t>
+          <t>Releases from Prison to Other Community Supervision That Is Not Probation or Parole</t>
         </is>
       </c>
       <c r="D165" t="inlineStr"/>
@@ -21194,7 +21193,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>No Additional Correctional Control</t>
+          <t>Releases from Prison to no Additional Correctional Control</t>
         </is>
       </c>
       <c r="D166" t="inlineStr"/>
@@ -21212,7 +21211,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Releases from Prison due to Death</t>
         </is>
       </c>
       <c r="D167" t="inlineStr"/>
@@ -21230,7 +21229,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Unknown Release</t>
+          <t>Other Releases from Prison</t>
         </is>
       </c>
       <c r="D168" t="inlineStr"/>
@@ -21248,7 +21247,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Other Release</t>
+          <t>Unknown Releases from Prison</t>
         </is>
       </c>
       <c r="D169" t="inlineStr"/>
@@ -21311,7 +21310,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21327,11 +21326,6 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>force_type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>value</t>
         </is>
       </c>
@@ -21342,129 +21336,15 @@
           <t>2021</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Restraint</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Verbal</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Weapon</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Restraint</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Verbal</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Weapon</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -21477,7 +21357,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21493,6 +21373,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>grievances_type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>value</t>
         </is>
       </c>
@@ -21503,15 +21388,181 @@
           <t>2021</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Living Conditions</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Personal Safety</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Discrimination, Racial Bias, or Religious Practices</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Access to Health Care</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Legal</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Other Grievance</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Unknown Grievance</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Living Conditions</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Personal Safety</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Discrimination, Racial Bias, or Religious Practices</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Access to Health Care</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Legal</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Other Grievance</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Unknown Grievance</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -21557,7 +21608,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>State Appropriation</t>
+          <t>State Appropriations</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -21596,7 +21647,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Contract Beds</t>
+          <t>Contract Beds (Funding)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -21635,7 +21686,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>State Appropriation</t>
+          <t>State Appropriations</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -21674,7 +21725,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Contract Beds</t>
+          <t>Contract Beds (Funding)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -21704,224 +21755,6 @@
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>year</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>grievances_type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Living Conditions</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Personal Safety</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Discrimination, Racial Bias, or Religious Practices</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Access to Health Care</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Legal</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Other Grievance</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Unknown Grievance</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Living Conditions</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Personal Safety</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Discrimination, Racial Bias, or Religious Practices</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Access to Health Care</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Legal</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Other Grievance</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Unknown Grievance</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -22066,7 +21899,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Contract Beds</t>
+          <t>Contract Beds (Expenses)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -22079,7 +21912,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Unknown Expenses</t>
+          <t>Other Expenses</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -22092,7 +21925,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Other Expenses</t>
+          <t>Unknown Expenses</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -22157,7 +21990,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Contract Beds</t>
+          <t>Contract Beds (Expenses)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -22170,7 +22003,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Unknown Expenses</t>
+          <t>Other Expenses</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -22183,7 +22016,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Other Expenses</t>
+          <t>Unknown Expenses</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -22305,7 +22138,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Clinical or Medical Staff</t>
+          <t>Clinical and Medical Staff</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -22331,7 +22164,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Vacant Positions (Any Staff Type)</t>
+          <t>Other Staff</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -22344,7 +22177,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Other Staff</t>
+          <t>Unknown Staff</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -22357,7 +22190,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Unknown Staff</t>
+          <t>Vacant Positions (Any Staff Type)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -22396,7 +22229,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Clinical or Medical Staff</t>
+          <t>Clinical and Medical Staff</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -22422,7 +22255,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Vacant Positions (Any Staff Type)</t>
+          <t>Other Staff</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -22435,7 +22268,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Other Staff</t>
+          <t>Unknown Staff</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -22448,7 +22281,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Unknown Staff</t>
+          <t>Vacant Positions (Any Staff Type)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -22511,7 +22344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22544,7 +22377,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>New Conviction</t>
+          <t>Readmissions for a New Conviction</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -22557,7 +22390,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Return from Probation</t>
+          <t>Readmissions from Probation</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -22570,7 +22403,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Return from Parole</t>
+          <t>Readmissions from Parole</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -22583,7 +22416,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Other Readmissions</t>
+          <t>Readmissions from Other Community Supervision</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -22596,7 +22429,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Unknown Post-Adjudication Readmission</t>
+          <t>Other Readmissions</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -22604,12 +22437,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>New Conviction</t>
+          <t>Unknown Readmissions</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -22622,7 +22455,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Return from Probation</t>
+          <t>Readmissions for a New Conviction</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -22635,7 +22468,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Return from Parole</t>
+          <t>Readmissions from Probation</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -22648,7 +22481,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Other Readmissions</t>
+          <t>Readmissions from Parole</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -22661,10 +22494,36 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Unknown Post-Adjudication Readmission</t>
+          <t>Readmissions from Other Community Supervision</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Other Readmissions</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Unknown Readmissions</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>